<commit_message>
Added documentary for KSZ8851
</commit_message>
<xml_diff>
--- a/MotorController/Datasheets/SAMC21/SAMC21_Pinout.xlsx
+++ b/MotorController/Datasheets/SAMC21/SAMC21_Pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\_work\MotorController\Datasheets\SAMC21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\_work\X2City\MotorController\Datasheets\SAMC21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE626390-C46A-468E-ACE8-2B5618BCDB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DF7D14-AFD1-45B1-95F1-A4FA964073A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28065" windowHeight="15885" xr2:uid="{B9B784E2-40E7-46A1-B6A9-A010A1749725}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B9B784E2-40E7-46A1-B6A9-A010A1749725}"/>
   </bookViews>
   <sheets>
     <sheet name="SAMC21" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="211">
   <si>
     <t>PORT_PA11</t>
   </si>
@@ -650,6 +650,15 @@
   </si>
   <si>
     <t>Duty_Ctrl</t>
+  </si>
+  <si>
+    <t>KSZ8851-&gt;CS</t>
+  </si>
+  <si>
+    <t>KSZ8851-&gt;INT</t>
+  </si>
+  <si>
+    <t>KSZ8851-&gt;RST</t>
   </si>
 </sst>
 </file>
@@ -673,7 +682,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -719,6 +728,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -850,6 +865,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -859,7 +876,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1306,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC464E6-459F-468A-901F-AD48611239EA}">
-  <dimension ref="A2:AD18"/>
+  <dimension ref="A2:AD31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,7 +1456,9 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="3"/>
+      <c r="N5" s="17" t="s">
+        <v>208</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>102</v>
       </c>
@@ -1559,13 +1577,13 @@
       <c r="I7" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="16" t="s">
         <v>147</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="19" t="s">
+      <c r="N7" s="16" t="s">
         <v>207</v>
       </c>
       <c r="Q7" s="8" t="s">
@@ -2036,7 +2054,9 @@
       <c r="N15" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="Q15" s="3"/>
+      <c r="Q15" s="17" t="s">
+        <v>210</v>
+      </c>
       <c r="R15" s="4" t="s">
         <v>127</v>
       </c>
@@ -2092,7 +2112,9 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="3"/>
-      <c r="Q16" s="3"/>
+      <c r="Q16" s="17" t="s">
+        <v>209</v>
+      </c>
       <c r="R16" s="6" t="s">
         <v>125</v>
       </c>
@@ -2119,7 +2141,7 @@
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>166</v>
       </c>
@@ -2145,7 +2167,7 @@
       <c r="M17" s="4"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>167</v>
       </c>
@@ -2170,6 +2192,11 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="3"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y31" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2216,12 +2243,12 @@
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="1" t="s">
         <v>26</v>
       </c>
@@ -2243,12 +2270,12 @@
       <c r="R3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="S3" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="18"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="20"/>
       <c r="W3" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Implemented ethernet debug frame
+ Restructuring of DeviceDriver
</commit_message>
<xml_diff>
--- a/MotorController/Datasheets/SAMC21/SAMC21_Pinout.xlsx
+++ b/MotorController/Datasheets/SAMC21/SAMC21_Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\_work\X2City\MotorController\Datasheets\SAMC21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DF7D14-AFD1-45B1-95F1-A4FA964073A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6604A70-D6D4-4765-B8A1-29C04EBF6F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B9B784E2-40E7-46A1-B6A9-A010A1749725}"/>
   </bookViews>
@@ -1325,7 +1325,7 @@
   <dimension ref="A2:AD31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>